<commit_message>
Updated UI, added logic for handling color click
</commit_message>
<xml_diff>
--- a/stm32_controller/assets/texts/texts.xlsx
+++ b/stm32_controller/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="65">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -189,6 +189,27 @@
   </si>
   <si>
     <t xml:space="preserve">Encendido&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789abcdef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789abcdef#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -1411,10 +1432,10 @@
       <c r="E4">
         <v>4</v>
       </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4"/>
+      <c r="F4"/>
+      <c r="G4" t="s">
+        <v>63</v>
+      </c>
       <c r="H4"/>
       <c r="I4"/>
       <c r="K4" s="4" t="s">
@@ -1446,10 +1467,10 @@
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5"/>
+      <c r="F5"/>
+      <c r="G5" t="s">
+        <v>63</v>
+      </c>
       <c r="H5"/>
       <c r="I5"/>
       <c r="K5" s="7" t="s">
@@ -1479,10 +1500,10 @@
       <c r="E6">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6"/>
+      <c r="F6"/>
+      <c r="G6" t="s">
+        <v>63</v>
+      </c>
       <c r="H6"/>
       <c r="I6"/>
       <c r="K6" s="7" t="s">
@@ -1629,9 +1650,6 @@
       <c r="F3" t="s">
         <v>47</v>
       </c>
-      <c r="G3" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="4">
       <c r="B4" t="s">
@@ -1647,32 +1665,10 @@
         <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" t="s">
-        <v>54</v>
-      </c>
-    </row>
+    <row r="5"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>